<commit_message>
chg: Update weather, update ordnance for D1.2
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAC Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAC Ordnance.xlsx
@@ -856,7 +856,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1041,7 +1041,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1416,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1466,7 +1466,7 @@
       <c r="R1" s="80"/>
       <c r="S1" s="80"/>
       <c r="T1" s="72" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="39.75" customHeight="1">
@@ -1580,7 +1580,7 @@
       <c r="R4" s="52"/>
       <c r="S4" s="52"/>
       <c r="T4" s="53">
-        <f>SUM(C4:C4)-SUM(D4:S4)</f>
+        <f t="shared" ref="T4:T19" si="0">SUM(C4:C4)-SUM(D4:S4)</f>
         <v>50</v>
       </c>
     </row>
@@ -1611,7 +1611,7 @@
       <c r="R5" s="57"/>
       <c r="S5" s="57"/>
       <c r="T5" s="53">
-        <f>SUM(C5:C5)-SUM(D5:S5)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -1642,7 +1642,7 @@
       <c r="R6" s="52"/>
       <c r="S6" s="52"/>
       <c r="T6" s="53">
-        <f>SUM(C6:C6)-SUM(D6:S6)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1656,7 +1656,9 @@
       <c r="C7" s="54">
         <v>15</v>
       </c>
-      <c r="D7" s="55"/>
+      <c r="D7" s="55">
+        <v>3</v>
+      </c>
       <c r="E7" s="56"/>
       <c r="F7" s="56"/>
       <c r="G7" s="56"/>
@@ -1673,8 +1675,8 @@
       <c r="R7" s="57"/>
       <c r="S7" s="57"/>
       <c r="T7" s="53">
-        <f>SUM(C7:C7)-SUM(D7:S7)</f>
-        <v>15</v>
+        <f t="shared" si="0"/>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:20">
@@ -1704,7 +1706,7 @@
       <c r="R8" s="52"/>
       <c r="S8" s="52"/>
       <c r="T8" s="71">
-        <f>SUM(C8:C8)-SUM(D8:S8)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
     </row>
@@ -1735,7 +1737,7 @@
       <c r="R9" s="57"/>
       <c r="S9" s="57"/>
       <c r="T9" s="71">
-        <f>SUM(C9:C9)-SUM(D9:S9)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
@@ -1749,7 +1751,9 @@
       <c r="C10" s="58">
         <v>20</v>
       </c>
-      <c r="D10" s="50"/>
+      <c r="D10" s="50">
+        <v>1</v>
+      </c>
       <c r="E10" s="51"/>
       <c r="F10" s="51"/>
       <c r="G10" s="51"/>
@@ -1766,8 +1770,8 @@
       <c r="R10" s="52"/>
       <c r="S10" s="52"/>
       <c r="T10" s="71">
-        <f>SUM(C10:C10)-SUM(D10:S10)</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:20">
@@ -1797,7 +1801,7 @@
       <c r="R11" s="57"/>
       <c r="S11" s="57"/>
       <c r="T11" s="71">
-        <f>SUM(C11:C11)-SUM(D11:S11)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -1828,7 +1832,7 @@
       <c r="R12" s="52"/>
       <c r="S12" s="52"/>
       <c r="T12" s="71">
-        <f>SUM(C12:C12)-SUM(D12:S12)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
@@ -1842,7 +1846,9 @@
       <c r="C13" s="54">
         <v>20</v>
       </c>
-      <c r="D13" s="55"/>
+      <c r="D13" s="55">
+        <v>4</v>
+      </c>
       <c r="E13" s="56"/>
       <c r="F13" s="56"/>
       <c r="G13" s="56"/>
@@ -1859,8 +1865,8 @@
       <c r="R13" s="57"/>
       <c r="S13" s="57"/>
       <c r="T13" s="71">
-        <f>SUM(C13:C13)-SUM(D13:S13)</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1890,7 +1896,7 @@
       <c r="R14" s="52"/>
       <c r="S14" s="52"/>
       <c r="T14" s="71">
-        <f>SUM(C14:C14)-SUM(D14:S14)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -1921,7 +1927,7 @@
       <c r="R15" s="57"/>
       <c r="S15" s="57"/>
       <c r="T15" s="71">
-        <f>SUM(C15:C15)-SUM(D15:S15)</f>
+        <f t="shared" si="0"/>
         <v>50</v>
       </c>
     </row>
@@ -1952,7 +1958,7 @@
       <c r="R16" s="52"/>
       <c r="S16" s="52"/>
       <c r="T16" s="71">
-        <f>SUM(C16:C16)-SUM(D16:S16)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1983,7 +1989,7 @@
       <c r="R17" s="57"/>
       <c r="S17" s="57"/>
       <c r="T17" s="71">
-        <f>SUM(C17:C17)-SUM(D17:S17)</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -1997,7 +2003,9 @@
       <c r="C18" s="61">
         <v>50</v>
       </c>
-      <c r="D18" s="62"/>
+      <c r="D18" s="62">
+        <v>14</v>
+      </c>
       <c r="E18" s="51"/>
       <c r="F18" s="51"/>
       <c r="G18" s="51"/>
@@ -2014,8 +2022,8 @@
       <c r="R18" s="52"/>
       <c r="S18" s="52"/>
       <c r="T18" s="53">
-        <f>SUM(C18:C18)-SUM(D18:S18)</f>
-        <v>50</v>
+        <f t="shared" si="0"/>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="15.75" thickBot="1">
@@ -2028,7 +2036,9 @@
       <c r="C19" s="65">
         <v>75</v>
       </c>
-      <c r="D19" s="66"/>
+      <c r="D19" s="66">
+        <v>6</v>
+      </c>
       <c r="E19" s="67"/>
       <c r="F19" s="67"/>
       <c r="G19" s="67"/>
@@ -2045,8 +2055,8 @@
       <c r="R19" s="69"/>
       <c r="S19" s="69"/>
       <c r="T19" s="70">
-        <f>SUM(C19:C19)-SUM(D19:S19)</f>
-        <v>75</v>
+        <f t="shared" si="0"/>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:20">

</xml_diff>

<commit_message>
chg: Updated ordnance and weather for D2.2
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAC Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAC Ordnance.xlsx
@@ -856,7 +856,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1041,7 +1041,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1416,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1466,7 +1466,7 @@
       <c r="R1" s="80"/>
       <c r="S1" s="80"/>
       <c r="T1" s="72" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="39.75" customHeight="1">
@@ -1823,7 +1823,9 @@
       <c r="E12" s="51">
         <v>4</v>
       </c>
-      <c r="F12" s="51"/>
+      <c r="F12" s="51">
+        <v>9</v>
+      </c>
       <c r="G12" s="51"/>
       <c r="H12" s="51"/>
       <c r="I12" s="51"/>
@@ -1839,7 +1841,7 @@
       <c r="S12" s="52"/>
       <c r="T12" s="71">
         <f t="shared" si="0"/>
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1856,7 +1858,9 @@
         <v>4</v>
       </c>
       <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
+      <c r="F13" s="56">
+        <v>2</v>
+      </c>
       <c r="G13" s="56"/>
       <c r="H13" s="56"/>
       <c r="I13" s="56"/>
@@ -1872,7 +1876,7 @@
       <c r="S13" s="57"/>
       <c r="T13" s="71">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:20">
@@ -1920,7 +1924,9 @@
       <c r="E15" s="56">
         <v>5</v>
       </c>
-      <c r="F15" s="56"/>
+      <c r="F15" s="56">
+        <v>2</v>
+      </c>
       <c r="G15" s="56"/>
       <c r="H15" s="56"/>
       <c r="I15" s="56"/>
@@ -1936,7 +1942,7 @@
       <c r="S15" s="57"/>
       <c r="T15" s="71">
         <f t="shared" si="0"/>
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -2017,7 +2023,9 @@
       <c r="E18" s="51">
         <v>5</v>
       </c>
-      <c r="F18" s="51"/>
+      <c r="F18" s="51">
+        <v>2</v>
+      </c>
       <c r="G18" s="51"/>
       <c r="H18" s="51"/>
       <c r="I18" s="51"/>
@@ -2033,7 +2041,7 @@
       <c r="S18" s="52"/>
       <c r="T18" s="53">
         <f t="shared" si="0"/>
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="15.75" thickBot="1">

</xml_diff>

<commit_message>
chg: Update ordnance for D3.1
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAC Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAC Ordnance.xlsx
@@ -856,7 +856,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1041,7 +1041,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1416,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1466,7 +1466,7 @@
       <c r="R1" s="80"/>
       <c r="S1" s="80"/>
       <c r="T1" s="72" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="39.75" customHeight="1">
@@ -1826,7 +1826,9 @@
       <c r="F12" s="51">
         <v>9</v>
       </c>
-      <c r="G12" s="51"/>
+      <c r="G12" s="51">
+        <v>1</v>
+      </c>
       <c r="H12" s="51"/>
       <c r="I12" s="51"/>
       <c r="J12" s="51"/>
@@ -1841,7 +1843,7 @@
       <c r="S12" s="52"/>
       <c r="T12" s="71">
         <f t="shared" si="0"/>
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:20">
@@ -1927,7 +1929,9 @@
       <c r="F15" s="56">
         <v>2</v>
       </c>
-      <c r="G15" s="56"/>
+      <c r="G15" s="56">
+        <v>4</v>
+      </c>
       <c r="H15" s="56"/>
       <c r="I15" s="56"/>
       <c r="J15" s="56"/>
@@ -1942,7 +1946,7 @@
       <c r="S15" s="57"/>
       <c r="T15" s="71">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:20">
@@ -2026,7 +2030,9 @@
       <c r="F18" s="51">
         <v>2</v>
       </c>
-      <c r="G18" s="51"/>
+      <c r="G18" s="51">
+        <v>4</v>
+      </c>
       <c r="H18" s="51"/>
       <c r="I18" s="51"/>
       <c r="J18" s="51"/>
@@ -2041,7 +2047,7 @@
       <c r="S18" s="52"/>
       <c r="T18" s="53">
         <f t="shared" si="0"/>
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:20" ht="15.75" thickBot="1">

</xml_diff>

<commit_message>
chg: Updated ordnance for D3.2
</commit_message>
<xml_diff>
--- a/MISSION INFORMATION/OPAC Ordnance.xlsx
+++ b/MISSION INFORMATION/OPAC Ordnance.xlsx
@@ -856,7 +856,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1041,7 +1041,7 @@
         <xdr:cNvPr id="2" name="TekstSylinder 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1416,7 +1416,7 @@
   <dimension ref="A1:T23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U14" sqref="U14"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1466,7 +1466,7 @@
       <c r="R1" s="80"/>
       <c r="S1" s="80"/>
       <c r="T1" s="72" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:20" ht="39.75" customHeight="1">
@@ -1829,7 +1829,9 @@
       <c r="G12" s="51">
         <v>1</v>
       </c>
-      <c r="H12" s="51"/>
+      <c r="H12" s="51">
+        <v>2</v>
+      </c>
       <c r="I12" s="51"/>
       <c r="J12" s="51"/>
       <c r="K12" s="51"/>
@@ -1843,7 +1845,7 @@
       <c r="S12" s="52"/>
       <c r="T12" s="71">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:20">

</xml_diff>